<commit_message>
Organized how some features will be regrouped.
</commit_message>
<xml_diff>
--- a/catagorical_feature_encoding.xlsx
+++ b/catagorical_feature_encoding.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saffra\Documents\senior_project\senior_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC2751D-7A4C-4313-923E-3EBC8EEAF1EA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BA1B41-91DB-4BA7-B8E2-EB9DE4AA4DD6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="1900" windowWidth="33050" windowHeight="16760" xr2:uid="{B6AC7372-773D-4A83-9E2E-E02C69B232EC}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
   <si>
     <t>AppVersion</t>
   </si>
@@ -199,13 +199,63 @@
   </si>
   <si>
     <t>These are categorical features that are considered worth_keeping_overall</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Should I keep this column?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I could group these but there wouldn't be a logical system because the city locations or size aren't identified. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Columns: </t>
+  </si>
+  <si>
+    <t>Values are from 3-72105</t>
+  </si>
+  <si>
+    <t>7 groups of 10,000</t>
+  </si>
+  <si>
+    <t>Values are from 3-70507</t>
+  </si>
+  <si>
+    <t>That will put about 3 million observations per group</t>
+  </si>
+  <si>
+    <t>That puts ~ 1mil observations per group and ~ 3 mil in the everything else group</t>
+  </si>
+  <si>
+    <t>"1.273",  "1.275", and everything else</t>
+  </si>
+  <si>
+    <t>2668, 2102, 1443, 2206, 585, 525, everything else</t>
+  </si>
+  <si>
+    <t>2000-2999, 3000-3999, everything else</t>
+  </si>
+  <si>
+    <t>2000 ~ 4.7 mil obs, 3 ~ 1.6 mil obs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,14 +290,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -560,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E937CDF3-F9D5-4A3D-939D-FB47B223C9B8}">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -572,7 +626,7 @@
     <col min="2" max="2" width="44.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="35.54296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="44.90625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.7265625" bestFit="1" customWidth="1"/>
@@ -580,7 +634,7 @@
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>54</v>
       </c>
@@ -596,67 +650,121 @@
       <c r="E1" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>42</v>
       </c>
       <c r="C2">
         <v>8921483</v>
       </c>
-      <c r="G2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>36</v>
       </c>
       <c r="C3">
         <v>107367</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>29</v>
       </c>
       <c r="C4">
         <v>50495</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>27</v>
       </c>
       <c r="C5">
         <v>28971</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>1</v>
       </c>
       <c r="C6">
         <v>8531</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>30</v>
       </c>
       <c r="C7">
         <v>3833</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>35</v>
       </c>
       <c r="C8">
         <v>3429</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>28</v>
       </c>
@@ -664,7 +772,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>18</v>
       </c>
@@ -672,7 +780,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>13</v>
       </c>
@@ -680,7 +788,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>40</v>
       </c>
@@ -688,7 +796,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>38</v>
       </c>
@@ -696,7 +804,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>32</v>
       </c>
@@ -704,7 +812,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>41</v>
       </c>
@@ -712,7 +820,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>37</v>
       </c>
@@ -985,12 +1093,26 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B49" t="s">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B49" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="1">
         <v>2</v>
+      </c>
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B50" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C50" s="3">
+        <f>SUM(C2:C49)</f>
+        <v>9128340</v>
+      </c>
+      <c r="D50">
+        <f>SUM(D2:D49)</f>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished deciding how to group catagorical features. Now need to code them.
</commit_message>
<xml_diff>
--- a/catagorical_feature_encoding.xlsx
+++ b/catagorical_feature_encoding.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saffra\Documents\senior_project\senior_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BA1B41-91DB-4BA7-B8E2-EB9DE4AA4DD6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F03C4C-B249-451C-918B-CB5420A5BE39}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="1900" windowWidth="33050" windowHeight="16760" xr2:uid="{B6AC7372-773D-4A83-9E2E-E02C69B232EC}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="93">
   <si>
     <t>AppVersion</t>
   </si>
@@ -238,6 +238,78 @@
   </si>
   <si>
     <t>2000 ~ 4.7 mil obs, 3 ~ 1.6 mil obs</t>
+  </si>
+  <si>
+    <t>142, 628, 554, everything else</t>
+  </si>
+  <si>
+    <t>2.6, 1.2, 1.1, 3.8 mil observations in each group (ordered)</t>
+  </si>
+  <si>
+    <t>16299, 17134, everything else</t>
+  </si>
+  <si>
+    <t>2.6, 3.9, 2.5 mil each (ordered)</t>
+  </si>
+  <si>
+    <t>17134, 16299, everything else</t>
+  </si>
+  <si>
+    <t>3.9, 2.5, 2.6 mil each (ordered)</t>
+  </si>
+  <si>
+    <t>277, then divide the remaining into two equal groups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">228, then divide the remaining into 7 more equal groups </t>
+  </si>
+  <si>
+    <t>Each group should have ~ 1.5 mil observations</t>
+  </si>
+  <si>
+    <t>Divide into groups of ~ 1 mil</t>
+  </si>
+  <si>
+    <t>4, 2.4, ~3 mil each</t>
+  </si>
+  <si>
+    <t>31, 34, divide the rest into 3 groups</t>
+  </si>
+  <si>
+    <t>3.1, 1, ~1+ mil each</t>
+  </si>
+  <si>
+    <t>8 groups of 1 mil each</t>
+  </si>
+  <si>
+    <t>10.0.17134.228, 10.0.17134.165, everything else divided into 6 more groups</t>
+  </si>
+  <si>
+    <t>Approx 1 mil each</t>
+  </si>
+  <si>
+    <t>1.1.15200.1, 1.1.15100.1, everything else</t>
+  </si>
+  <si>
+    <t>3.8, 3.6, ~1 mil each</t>
+  </si>
+  <si>
+    <t>10.0.0.0, everything else</t>
+  </si>
+  <si>
+    <t>8.6, &lt;1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.2 mil are notebook. Everything else could be grouped into another massive bundle or it could be sorted better. </t>
+  </si>
+  <si>
+    <t>notebook, everything else</t>
+  </si>
+  <si>
+    <t>27, 18,  everything else</t>
+  </si>
+  <si>
+    <t>4.1, 1.7, ~3 mil each</t>
   </si>
 </sst>
 </file>
@@ -264,12 +336,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -294,11 +372,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -616,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E937CDF3-F9D5-4A3D-939D-FB47B223C9B8}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -626,7 +705,7 @@
     <col min="2" max="2" width="44.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="35.54296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="44.90625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.7265625" bestFit="1" customWidth="1"/>
@@ -675,6 +754,12 @@
       <c r="C3">
         <v>107367</v>
       </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>82</v>
+      </c>
       <c r="F3" t="s">
         <v>58</v>
       </c>
@@ -771,6 +856,15 @@
       <c r="C9">
         <v>713</v>
       </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
@@ -779,6 +873,15 @@
       <c r="C10">
         <v>664</v>
       </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
@@ -787,13 +890,31 @@
       <c r="C11">
         <v>469</v>
       </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C12">
         <v>304</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -803,6 +924,12 @@
       <c r="C13">
         <v>293</v>
       </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
@@ -811,6 +938,15 @@
       <c r="C14">
         <v>285</v>
       </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
@@ -819,6 +955,15 @@
       <c r="C15">
         <v>276</v>
       </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
@@ -827,269 +972,412 @@
       <c r="C16">
         <v>222</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="F16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>31</v>
       </c>
       <c r="C17">
         <v>165</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>33</v>
       </c>
       <c r="C18">
         <v>147</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>110</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>15</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B20" t="s">
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B20" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C20">
         <v>76</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>17</v>
       </c>
       <c r="C21">
         <v>70</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>85</v>
+      </c>
+      <c r="F21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>20</v>
       </c>
       <c r="C22">
         <v>58</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>3</v>
       </c>
       <c r="C23">
         <v>53</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B24" t="s">
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D24" s="1">
+        <v>3</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>10</v>
       </c>
       <c r="C25">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>9</v>
       </c>
       <c r="C26">
         <v>32</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D26">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>12</v>
       </c>
       <c r="C27">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D27">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>24</v>
       </c>
       <c r="C28">
         <v>22</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D28">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>47</v>
       </c>
       <c r="C29">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>45</v>
       </c>
       <c r="C30">
         <v>14</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D30">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>7</v>
       </c>
       <c r="C31">
         <v>13</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D31">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>15</v>
       </c>
       <c r="C32">
         <v>11</v>
       </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D32">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>5</v>
       </c>
       <c r="C33">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>26</v>
       </c>
       <c r="C34">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D34">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>11</v>
       </c>
       <c r="C35">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>19</v>
       </c>
       <c r="C36">
         <v>9</v>
       </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D36">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>34</v>
       </c>
       <c r="C37">
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D37">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>46</v>
       </c>
       <c r="C38">
         <v>8</v>
       </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D38">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>23</v>
       </c>
       <c r="C39">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D39">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>25</v>
       </c>
       <c r="C40">
         <v>7</v>
       </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D40">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>2</v>
       </c>
       <c r="C41">
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D41">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>14</v>
       </c>
       <c r="C42">
         <v>6</v>
       </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D42">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>6</v>
       </c>
       <c r="C43">
         <v>5</v>
       </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>16</v>
       </c>
       <c r="C44">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>21</v>
       </c>
       <c r="C45">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>4</v>
       </c>
       <c r="C46">
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>8</v>
       </c>
       <c r="C47">
         <v>3</v>
       </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>22</v>
       </c>
       <c r="C48">
+        <v>3</v>
+      </c>
+      <c r="D48">
         <v>3</v>
       </c>
     </row>
@@ -1100,7 +1388,9 @@
       <c r="C49" s="1">
         <v>2</v>
       </c>
-      <c r="D49" s="1"/>
+      <c r="D49" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B50" s="2" t="s">
@@ -1112,7 +1402,7 @@
       </c>
       <c r="D50">
         <f>SUM(D2:D49)</f>
-        <v>42</v>
+        <v>392</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished organizing the data and now started one hot encoding the categorical features.
</commit_message>
<xml_diff>
--- a/catagorical_feature_encoding.xlsx
+++ b/catagorical_feature_encoding.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saffra\Documents\senior_project\senior_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F03C4C-B249-451C-918B-CB5420A5BE39}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E96D2ED-A7EB-4A78-AC58-716076BD4DF3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="1900" windowWidth="33050" windowHeight="16760" xr2:uid="{B6AC7372-773D-4A83-9E2E-E02C69B232EC}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="98">
   <si>
     <t>AppVersion</t>
   </si>
@@ -225,9 +225,6 @@
     <t>That will put about 3 million observations per group</t>
   </si>
   <si>
-    <t>That puts ~ 1mil observations per group and ~ 3 mil in the everything else group</t>
-  </si>
-  <si>
     <t>"1.273",  "1.275", and everything else</t>
   </si>
   <si>
@@ -240,12 +237,6 @@
     <t>2000 ~ 4.7 mil obs, 3 ~ 1.6 mil obs</t>
   </si>
   <si>
-    <t>142, 628, 554, everything else</t>
-  </si>
-  <si>
-    <t>2.6, 1.2, 1.1, 3.8 mil observations in each group (ordered)</t>
-  </si>
-  <si>
     <t>16299, 17134, everything else</t>
   </si>
   <si>
@@ -267,9 +258,6 @@
     <t>Each group should have ~ 1.5 mil observations</t>
   </si>
   <si>
-    <t>Divide into groups of ~ 1 mil</t>
-  </si>
-  <si>
     <t>4, 2.4, ~3 mil each</t>
   </si>
   <si>
@@ -310,6 +298,33 @@
   </si>
   <si>
     <t>4.1, 1.7, ~3 mil each</t>
+  </si>
+  <si>
+    <t>137, 117, everything else</t>
+  </si>
+  <si>
+    <t>1.5 mil</t>
+  </si>
+  <si>
+    <t>Not Working</t>
+  </si>
+  <si>
+    <t>Delete?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete </t>
+  </si>
+  <si>
+    <t>Anything over 800k gets its own group</t>
+  </si>
+  <si>
+    <t>Anything less than 100k grouped together?</t>
+  </si>
+  <si>
+    <t>142, 628, 554, 355, 556, everything else</t>
+  </si>
+  <si>
+    <t>Left alone</t>
   </si>
 </sst>
 </file>
@@ -336,7 +351,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -345,7 +360,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -372,12 +399,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -695,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E937CDF3-F9D5-4A3D-939D-FB47B223C9B8}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -737,44 +769,48 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C2">
         <v>8921483</v>
       </c>
+      <c r="E2" s="4"/>
       <c r="F2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C3">
         <v>107367</v>
       </c>
-      <c r="D3">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>82</v>
+      <c r="E3" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="F3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
+      <c r="A4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>29</v>
       </c>
       <c r="C4">
         <v>50495</v>
       </c>
-      <c r="D4">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>61</v>
       </c>
       <c r="F4" t="s">
@@ -782,16 +818,16 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
+      <c r="A5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C5">
         <v>28971</v>
       </c>
-      <c r="D5">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>61</v>
       </c>
       <c r="F5" t="s">
@@ -799,6 +835,9 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>91</v>
+      </c>
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -808,14 +847,17 @@
       <c r="D6">
         <v>3</v>
       </c>
-      <c r="E6" t="s">
-        <v>65</v>
+      <c r="E6" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="F6" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>53</v>
+      </c>
       <c r="B7" t="s">
         <v>30</v>
       </c>
@@ -825,31 +867,37 @@
       <c r="D7">
         <v>7</v>
       </c>
-      <c r="E7" t="s">
-        <v>66</v>
+      <c r="E7" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="F7" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
+      <c r="A8" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C8">
         <v>3429</v>
       </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="E8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" t="s">
         <v>67</v>
       </c>
-      <c r="F8" t="s">
-        <v>68</v>
+      <c r="G8" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>53</v>
+      </c>
       <c r="B9" t="s">
         <v>28</v>
       </c>
@@ -859,14 +907,17 @@
       <c r="D9">
         <v>4</v>
       </c>
-      <c r="E9" t="s">
-        <v>69</v>
+      <c r="E9" s="4" t="s">
+        <v>96</v>
       </c>
       <c r="F9" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>53</v>
+      </c>
       <c r="B10" t="s">
         <v>18</v>
       </c>
@@ -876,31 +927,34 @@
       <c r="D10">
         <v>3</v>
       </c>
-      <c r="E10" t="s">
-        <v>71</v>
+      <c r="E10" s="9" t="s">
+        <v>68</v>
       </c>
       <c r="F10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
+      <c r="A11" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C11">
         <v>469</v>
       </c>
-      <c r="D11">
-        <v>8</v>
-      </c>
-      <c r="E11" t="s">
-        <v>83</v>
+      <c r="E11" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="F11" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>53</v>
+      </c>
       <c r="B12" s="4" t="s">
         <v>40</v>
       </c>
@@ -910,62 +964,68 @@
       <c r="D12">
         <v>3</v>
       </c>
-      <c r="E12" t="s">
-        <v>73</v>
+      <c r="E12" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="F12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
+      <c r="A13" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C13">
         <v>293</v>
       </c>
-      <c r="D13">
-        <v>3</v>
-      </c>
-      <c r="E13" t="s">
-        <v>75</v>
+      <c r="E13" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
+      <c r="A14" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>32</v>
       </c>
       <c r="C14">
         <v>285</v>
       </c>
-      <c r="D14">
-        <v>8</v>
-      </c>
-      <c r="E14" t="s">
-        <v>76</v>
+      <c r="E14" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="F14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
+      <c r="A15" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>41</v>
       </c>
       <c r="C15">
         <v>276</v>
       </c>
-      <c r="D15">
-        <v>8</v>
-      </c>
-      <c r="E15" t="s">
-        <v>76</v>
+      <c r="E15" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="F15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="s">
+        <v>53</v>
+      </c>
       <c r="B16" t="s">
         <v>37</v>
       </c>
@@ -973,13 +1033,17 @@
         <v>222</v>
       </c>
       <c r="D16">
-        <v>8</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="E16" s="4"/>
       <c r="F16" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
+        <v>53</v>
+      </c>
       <c r="B17" t="s">
         <v>31</v>
       </c>
@@ -989,14 +1053,17 @@
       <c r="D17">
         <v>3</v>
       </c>
-      <c r="E17" t="s">
-        <v>73</v>
+      <c r="E17" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="F17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
+        <v>53</v>
+      </c>
       <c r="B18" t="s">
         <v>33</v>
       </c>
@@ -1007,10 +1074,10 @@
         <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F18" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -1032,23 +1099,26 @@
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B20" s="4" t="s">
+      <c r="A20" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>44</v>
       </c>
       <c r="C20">
         <v>76</v>
       </c>
-      <c r="D20">
-        <v>3</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>73</v>
+      <c r="E20" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="F20" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>91</v>
+      </c>
       <c r="B21" t="s">
         <v>17</v>
       </c>
@@ -1059,13 +1129,16 @@
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F21" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>91</v>
+      </c>
       <c r="B22" t="s">
         <v>20</v>
       </c>
@@ -1076,13 +1149,16 @@
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F22" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>53</v>
+      </c>
       <c r="B23" t="s">
         <v>3</v>
       </c>
@@ -1093,14 +1169,16 @@
         <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F23" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="1"/>
+      <c r="A24" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
@@ -1111,10 +1189,10 @@
         <v>3</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
@@ -1402,7 +1480,7 @@
       </c>
       <c r="D50">
         <f>SUM(D2:D49)</f>
-        <v>392</v>
+        <v>551</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tried to turn categorical features in to factors but not much luck. May need to significantly slim down the data.
</commit_message>
<xml_diff>
--- a/catagorical_feature_encoding.xlsx
+++ b/catagorical_feature_encoding.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saffra\Documents\senior_project\senior_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E96D2ED-A7EB-4A78-AC58-716076BD4DF3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1C0BB3-7CAE-4922-B39D-876A51C08F58}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="1900" windowWidth="33050" windowHeight="16760" xr2:uid="{B6AC7372-773D-4A83-9E2E-E02C69B232EC}"/>
   </bookViews>
@@ -728,7 +728,7 @@
   <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>